<commit_message>
Bangalore Batch Module 1 MTT question added
</commit_message>
<xml_diff>
--- a/Bangalore_And_Bhubaneshwar (23rd_Sep) Batch_Java_Full_Stack/Bangalore/MPT_MTT/Module 1/JavaFullStack-Module1_Java_SQL_JDBC_MTT-Assessment.xlsx
+++ b/Bangalore_And_Bhubaneshwar (23rd_Sep) Batch_Java_Full_Stack/Bangalore/MPT_MTT/Module 1/JavaFullStack-Module1_Java_SQL_JDBC_MTT-Assessment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Company\CG\JSpiders-CG-HTDProgram\Bangalore_And_Bhubaneshwar (23rd_Sep) Batch_Java_Full_Stack\Bangalore\MPT_MTT\Module 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Company\CG\JSpiders-CG-HTDProgram\Bangalore_And_Bhubaneshwar (23rd_Sep) Batch_Java_Full_Stack\Bhubaneswar\MPT_MTT\Module 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="203">
   <si>
     <t>Skill</t>
   </si>
@@ -560,7 +560,40 @@
     <t>String() &amp; StringBuffer()</t>
   </si>
   <si>
+    <t>Which of following annotation/s belong to Junit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  '@TestFactory' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@BeforeAll' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@AfterAll' </t>
+  </si>
+  <si>
+    <t>@Component'</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
     <t>JDBC</t>
+  </si>
+  <si>
+    <t>Which type of Statement can execute parameterized queries?</t>
+  </si>
+  <si>
+    <t>PreparedStatement</t>
+  </si>
+  <si>
+    <t>ParameterizedStatement and CallableStatement</t>
+  </si>
+  <si>
+    <t>ParameterizedStatement</t>
+  </si>
+  <si>
+    <t>All kinds of Statements (i.e. which implement a sub interface of Statement)</t>
   </si>
   <si>
     <t>In order to transfer data between a database and an application written in the Java programming language, the JDBC API provides which of these methods?</t>
@@ -704,21 +737,6 @@
   </si>
   <si>
     <t>Self Join</t>
-  </si>
-  <si>
-    <t>Which type of Statement can execute parameterized queries?</t>
-  </si>
-  <si>
-    <t>PreparedStatement</t>
-  </si>
-  <si>
-    <t>ParameterizedStatement and CallableStatement</t>
-  </si>
-  <si>
-    <t>ParameterizedStatement</t>
-  </si>
-  <si>
-    <t>All kinds of Statements (i.e. which implement a sub interface of Statement)</t>
   </si>
 </sst>
 </file>
@@ -787,6 +805,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="13"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -798,19 +829,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -879,7 +897,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -973,13 +991,25 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1003,7 +1033,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1011,12 +1041,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1299,9 +1323,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="A31" sqref="A31:XFD40"/>
     </sheetView>
   </sheetViews>
@@ -2190,7 +2214,7 @@
     </row>
     <row r="31" spans="1:9" s="34" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>17</v>
@@ -2198,20 +2222,20 @@
       <c r="C31" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="52" t="s">
-        <v>192</v>
-      </c>
-      <c r="E31" s="53" t="s">
-        <v>193</v>
-      </c>
-      <c r="F31" s="53" t="s">
-        <v>194</v>
-      </c>
-      <c r="G31" s="53" t="s">
-        <v>195</v>
-      </c>
-      <c r="H31" s="53" t="s">
-        <v>196</v>
+      <c r="D31" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="F31" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="G31" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="H31" s="42" t="s">
+        <v>158</v>
       </c>
       <c r="I31" s="4">
         <v>1</v>
@@ -2219,7 +2243,7 @@
     </row>
     <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>17</v>
@@ -2228,19 +2252,19 @@
         <v>22</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="I32" s="4">
         <v>4</v>
@@ -2248,7 +2272,7 @@
     </row>
     <row r="33" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>17</v>
@@ -2257,19 +2281,19 @@
         <v>10</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="I33" s="4">
         <v>1</v>
@@ -2277,7 +2301,7 @@
     </row>
     <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>17</v>
@@ -2286,16 +2310,16 @@
         <v>10</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>33</v>
@@ -2306,7 +2330,7 @@
     </row>
     <row r="35" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>9</v>
@@ -2315,16 +2339,16 @@
         <v>10</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>21</v>
@@ -2333,149 +2357,178 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="43" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="B36" s="39" t="s">
+    <row r="36" spans="1:9" s="47" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="B36" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="E36" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="F36" s="40" t="s">
-        <v>169</v>
-      </c>
-      <c r="G36" s="41" t="s">
-        <v>170</v>
-      </c>
-      <c r="H36" s="40" t="s">
-        <v>171</v>
-      </c>
-      <c r="I36" s="42">
+      <c r="C36" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="E36" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="F36" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="G36" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="H36" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="I36" s="46">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="47" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="B37" s="44" t="s">
+    <row r="37" spans="1:9" s="51" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="B37" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="44" t="s">
-        <v>172</v>
-      </c>
-      <c r="E37" s="44" t="s">
-        <v>173</v>
-      </c>
-      <c r="F37" s="44" t="s">
-        <v>174</v>
-      </c>
-      <c r="G37" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="H37" s="45" t="s">
-        <v>176</v>
-      </c>
-      <c r="I37" s="46">
+      <c r="C37" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="E37" s="48" t="s">
+        <v>184</v>
+      </c>
+      <c r="F37" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="G37" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="H37" s="49" t="s">
+        <v>187</v>
+      </c>
+      <c r="I37" s="50">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="50" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="B38" s="48" t="s">
+    <row r="38" spans="1:9" s="54" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="B38" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="48" t="s">
+      <c r="C38" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="E38" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="F38" s="52" t="s">
+        <v>190</v>
+      </c>
+      <c r="G38" s="53" t="s">
+        <v>191</v>
+      </c>
+      <c r="H38" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="I38" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="51" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="43" t="s">
         <v>177</v>
       </c>
-      <c r="E38" s="48" t="s">
-        <v>178</v>
-      </c>
-      <c r="F38" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="G38" s="49" t="s">
-        <v>180</v>
-      </c>
-      <c r="H38" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="I38" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="47" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="B39" s="48" t="s">
+      <c r="B39" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="51" t="s">
-        <v>182</v>
-      </c>
-      <c r="E39" s="45" t="s">
-        <v>183</v>
-      </c>
-      <c r="F39" s="45" t="s">
-        <v>184</v>
-      </c>
-      <c r="G39" s="45" t="s">
-        <v>185</v>
-      </c>
-      <c r="H39" s="45" t="s">
-        <v>186</v>
-      </c>
-      <c r="I39" s="46">
+      <c r="C39" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="E39" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="F39" s="49" t="s">
+        <v>195</v>
+      </c>
+      <c r="G39" s="49" t="s">
+        <v>196</v>
+      </c>
+      <c r="H39" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="I39" s="50">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="47" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="B40" s="44" t="s">
+    <row r="40" spans="1:9" s="51" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="51" t="s">
-        <v>187</v>
-      </c>
-      <c r="E40" s="45" t="s">
-        <v>188</v>
-      </c>
-      <c r="F40" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="G40" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="H40" s="45" t="s">
-        <v>191</v>
-      </c>
-      <c r="I40" s="46">
+      <c r="C40" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="55" t="s">
+        <v>198</v>
+      </c>
+      <c r="E40" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="F40" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="G40" s="49" t="s">
+        <v>201</v>
+      </c>
+      <c r="H40" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="I40" s="50">
         <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F41" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="G41" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="H41" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Few questions added for Exception and Threads in MTT for all the Batches
</commit_message>
<xml_diff>
--- a/Bangalore_And_Bhubaneshwar (23rd_Sep) Batch_Java_Full_Stack/Bangalore/MPT_MTT/Module 1/JavaFullStack-Module1_Java_SQL_JDBC_MTT-Assessment.xlsx
+++ b/Bangalore_And_Bhubaneshwar (23rd_Sep) Batch_Java_Full_Stack/Bangalore/MPT_MTT/Module 1/JavaFullStack-Module1_Java_SQL_JDBC_MTT-Assessment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Company\CG\JSpiders-CG-HTDProgram\Bangalore_And_Bhubaneshwar (23rd_Sep) Batch_Java_Full_Stack\Bhubaneswar\MPT_MTT\Module 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Company\CG\JSpiders-CG-HTDProgram\Bangalore_And_Bhubaneshwar (23rd_Sep) Batch_Java_Full_Stack\Bangalore\MPT_MTT\Module 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="205">
   <si>
     <t>Skill</t>
   </si>
@@ -395,51 +395,6 @@
     <t>all of the mentioned</t>
   </si>
   <si>
-    <t>Which among the following is not a necessary condition for constructors?</t>
-  </si>
-  <si>
-    <t>Its name must be same as that of class</t>
-  </si>
-  <si>
-    <t>It must not have any return type</t>
-  </si>
-  <si>
-    <t>It must contain a definition body</t>
-  </si>
-  <si>
-    <t>It can contains arguments</t>
-  </si>
-  <si>
-    <t>If data members are private, what can we do to access them from the class object?</t>
-  </si>
-  <si>
-    <t>Create public member functions to access those data members</t>
-  </si>
-  <si>
-    <t>Create private member functions to access those data members</t>
-  </si>
-  <si>
-    <t>Create protected member functions to access those data members</t>
-  </si>
-  <si>
-    <t>Private data members can never be accessed from outside the class</t>
-  </si>
-  <si>
-    <t>Encapsulation and abstraction differ as:</t>
-  </si>
-  <si>
-    <t>Binding and Hiding respectively</t>
-  </si>
-  <si>
-    <t>Hiding and Binding respectively</t>
-  </si>
-  <si>
-    <t>Can be used any way</t>
-  </si>
-  <si>
-    <t>Hiding and hiding respectively</t>
-  </si>
-  <si>
     <t>Which among the following is not a method of Throwable class?</t>
   </si>
   <si>
@@ -737,6 +692,101 @@
   </si>
   <si>
     <t>Self Join</t>
+  </si>
+  <si>
+    <t>Exceptions</t>
+  </si>
+  <si>
+    <t>class Test extends Exception { }
+class Main {
+   public static void main(String args[]) { 
+      try {
+         throw new Test();
+      }
+      catch(Test t) {
+         System.out.println("Got the Test Exception");
+      }
+      finally {
+         System.out.println("Inside finally block ");
+      }
+  }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Got the Test Exception
+Inside finally block </t>
+  </si>
+  <si>
+    <t>Got the Test Exception</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inside finally block </t>
+  </si>
+  <si>
+    <t>Compiler Error</t>
+  </si>
+  <si>
+    <t>Thread</t>
+  </si>
+  <si>
+    <t>class MultithreadedPrograming
+    {
+        public static void main(String args[])
+        {
+            Thread t = Thread.currentThread();
+            t.setName("New Thread");
+            System.out.println(t);        
+        }
+    }</t>
+  </si>
+  <si>
+    <t>Thread[5,main].</t>
+  </si>
+  <si>
+    <t>Thread[New Thread,5].</t>
+  </si>
+  <si>
+    <t>Thread[main,5,main].</t>
+  </si>
+  <si>
+    <t>Thread[New Thread,5,main].</t>
+  </si>
+  <si>
+    <t>class Test
+{
+    public static void main (String[] args)
+    {
+        try
+        {
+            int a = 0;
+            System.out.println ("a = " + a);
+            int b = 20 / a;
+            System.out.println ("b = " + b);
+        }
+        catch(ArithmeticException e)
+        {
+            System.out.println ("Divide by zero error");
+        }
+        finally
+        {
+            System.out.println ("inside the finally block");
+        }
+    }
+}</t>
+  </si>
+  <si>
+    <t>Compile error</t>
+  </si>
+  <si>
+    <t>a = 0
+Divide by zero error
+inside the finally block</t>
+  </si>
+  <si>
+    <t>A = 0</t>
+  </si>
+  <si>
+    <t>inside the finally block</t>
   </si>
 </sst>
 </file>
@@ -897,7 +947,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1041,6 +1091,38 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1325,8 +1407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD40"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,91 +2004,91 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="I21" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="I22" s="27">
+    <row r="21" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+      <c r="A21" s="58" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="E21" s="60" t="s">
+        <v>190</v>
+      </c>
+      <c r="F21" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="G21" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="H21" s="58" t="s">
+        <v>193</v>
+      </c>
+      <c r="I21" s="57">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="I23" s="27">
-        <v>1</v>
+    <row r="22" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A22" s="63" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="E22" s="63" t="s">
+        <v>196</v>
+      </c>
+      <c r="F22" s="63" t="s">
+        <v>197</v>
+      </c>
+      <c r="G22" s="63" t="s">
+        <v>198</v>
+      </c>
+      <c r="H22" s="63" t="s">
+        <v>199</v>
+      </c>
+      <c r="I22" s="63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="375" x14ac:dyDescent="0.25">
+      <c r="A23" s="64" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="66" t="s">
+        <v>200</v>
+      </c>
+      <c r="E23" s="64" t="s">
+        <v>201</v>
+      </c>
+      <c r="F23" s="66" t="s">
+        <v>202</v>
+      </c>
+      <c r="G23" s="64" t="s">
+        <v>203</v>
+      </c>
+      <c r="H23" s="64" t="s">
+        <v>204</v>
+      </c>
+      <c r="I23" s="67">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2020,19 +2102,19 @@
         <v>10</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="H24" s="35" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="I24" s="27">
         <v>4</v>
@@ -2049,19 +2131,19 @@
         <v>10</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="I25" s="27">
         <v>2</v>
@@ -2078,19 +2160,19 @@
         <v>10</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="I26" s="27">
         <v>3</v>
@@ -2107,19 +2189,19 @@
         <v>10</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="I27" s="27">
         <v>1</v>
@@ -2136,19 +2218,19 @@
         <v>10</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="I28" s="27">
         <v>3</v>
@@ -2165,19 +2247,19 @@
         <v>10</v>
       </c>
       <c r="D29" s="36" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="E29" s="37" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="F29" s="37" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="G29" s="37" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="H29" s="37" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="I29" s="38">
         <v>3</v>
@@ -2194,16 +2276,16 @@
         <v>10</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>86</v>
@@ -2214,7 +2296,7 @@
     </row>
     <row r="31" spans="1:9" s="34" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>17</v>
@@ -2223,19 +2305,19 @@
         <v>10</v>
       </c>
       <c r="D31" s="41" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="E31" s="42" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="F31" s="42" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="G31" s="42" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="H31" s="42" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="I31" s="4">
         <v>1</v>
@@ -2243,7 +2325,7 @@
     </row>
     <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>17</v>
@@ -2252,19 +2334,19 @@
         <v>22</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="I32" s="4">
         <v>4</v>
@@ -2272,7 +2354,7 @@
     </row>
     <row r="33" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>17</v>
@@ -2281,19 +2363,19 @@
         <v>10</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="I33" s="4">
         <v>1</v>
@@ -2301,7 +2383,7 @@
     </row>
     <row r="34" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>17</v>
@@ -2310,16 +2392,16 @@
         <v>10</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>33</v>
@@ -2330,7 +2412,7 @@
     </row>
     <row r="35" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>9</v>
@@ -2339,16 +2421,16 @@
         <v>10</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>21</v>
@@ -2359,7 +2441,7 @@
     </row>
     <row r="36" spans="1:9" s="47" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="43" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B36" s="43" t="s">
         <v>9</v>
@@ -2368,19 +2450,19 @@
         <v>10</v>
       </c>
       <c r="D36" s="43" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="E36" s="44" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="F36" s="44" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="G36" s="45" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="H36" s="44" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="I36" s="46">
         <v>3</v>
@@ -2388,7 +2470,7 @@
     </row>
     <row r="37" spans="1:9" s="51" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="43" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B37" s="48" t="s">
         <v>9</v>
@@ -2397,19 +2479,19 @@
         <v>10</v>
       </c>
       <c r="D37" s="48" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="E37" s="48" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="F37" s="48" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="G37" s="49" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="H37" s="49" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="I37" s="50">
         <v>1</v>
@@ -2417,7 +2499,7 @@
     </row>
     <row r="38" spans="1:9" s="54" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="43" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B38" s="52" t="s">
         <v>9</v>
@@ -2426,19 +2508,19 @@
         <v>10</v>
       </c>
       <c r="D38" s="52" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="E38" s="52" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="F38" s="52" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="G38" s="53" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="H38" s="52" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="I38" s="46">
         <v>1</v>
@@ -2446,7 +2528,7 @@
     </row>
     <row r="39" spans="1:9" s="51" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="43" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B39" s="52" t="s">
         <v>9</v>
@@ -2455,19 +2537,19 @@
         <v>10</v>
       </c>
       <c r="D39" s="55" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="E39" s="49" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="F39" s="49" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="G39" s="49" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="H39" s="49" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="I39" s="50">
         <v>4</v>
@@ -2475,7 +2557,7 @@
     </row>
     <row r="40" spans="1:9" s="51" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="43" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B40" s="48" t="s">
         <v>17</v>
@@ -2484,19 +2566,19 @@
         <v>10</v>
       </c>
       <c r="D40" s="55" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="E40" s="49" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="F40" s="49" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="G40" s="49" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="H40" s="49" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="I40" s="50">
         <v>4</v>
@@ -2513,22 +2595,22 @@
         <v>22</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="F41" s="39" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="G41" s="40" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="H41" s="40" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>